<commit_message>
Cleaning up example specification files
</commit_message>
<xml_diff>
--- a/model_specifications/test_parameters_chl.xlsx
+++ b/model_specifications/test_parameters_chl.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{542F22AF-E250-4AF5-9A5B-382E3C11F389}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="19392" windowHeight="10392" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="transitions" sheetId="1" r:id="rId1"/>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="47">
   <si>
     <t>start_state</t>
   </si>
@@ -161,12 +162,15 @@
   </si>
   <si>
     <t>Palliative_remission</t>
+  </si>
+  <si>
+    <t>static</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -477,23 +481,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="26" customWidth="1"/>
-    <col min="2" max="2" width="26.140625" customWidth="1"/>
-    <col min="3" max="3" width="17.140625" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" customWidth="1"/>
+    <col min="2" max="2" width="26.15625" customWidth="1"/>
+    <col min="3" max="3" width="17.15625" customWidth="1"/>
+    <col min="4" max="4" width="18.41796875" customWidth="1"/>
+    <col min="5" max="5" width="12.83984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -510,7 +514,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>28</v>
       </c>
@@ -524,7 +528,7 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -538,7 +542,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>28</v>
       </c>
@@ -552,7 +556,7 @@
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>28</v>
       </c>
@@ -566,7 +570,7 @@
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -580,7 +584,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>30</v>
       </c>
@@ -594,7 +598,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>30</v>
       </c>
@@ -608,7 +612,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>29</v>
       </c>
@@ -622,7 +626,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>29</v>
       </c>
@@ -636,7 +640,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>29</v>
       </c>
@@ -650,7 +654,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>29</v>
       </c>
@@ -664,7 +668,7 @@
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>29</v>
       </c>
@@ -678,7 +682,7 @@
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>35</v>
       </c>
@@ -692,7 +696,7 @@
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
         <v>35</v>
       </c>
@@ -706,7 +710,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
         <v>35</v>
       </c>
@@ -720,7 +724,7 @@
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
         <v>35</v>
       </c>
@@ -734,7 +738,7 @@
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
         <v>35</v>
       </c>
@@ -748,7 +752,7 @@
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
         <v>31</v>
       </c>
@@ -762,7 +766,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
         <v>31</v>
       </c>
@@ -776,7 +780,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
         <v>31</v>
       </c>
@@ -790,7 +794,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
         <v>31</v>
       </c>
@@ -804,7 +808,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
         <v>39</v>
       </c>
@@ -818,7 +822,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
         <v>39</v>
       </c>
@@ -832,7 +836,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
         <v>39</v>
       </c>
@@ -846,7 +850,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
         <v>39</v>
       </c>
@@ -860,7 +864,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
         <v>39</v>
       </c>
@@ -874,7 +878,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
         <v>38</v>
       </c>
@@ -888,7 +892,7 @@
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
         <v>38</v>
       </c>
@@ -902,7 +906,7 @@
         <v>0.27500000000000002</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
         <v>38</v>
       </c>
@@ -916,7 +920,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
         <v>38</v>
       </c>
@@ -930,7 +934,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
         <v>38</v>
       </c>
@@ -944,7 +948,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
         <v>36</v>
       </c>
@@ -958,7 +962,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
         <v>36</v>
       </c>
@@ -972,7 +976,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
         <v>36</v>
       </c>
@@ -986,7 +990,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" t="s">
         <v>36</v>
       </c>
@@ -1000,7 +1004,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="s">
         <v>41</v>
       </c>
@@ -1014,7 +1018,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="s">
         <v>41</v>
       </c>
@@ -1028,7 +1032,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" t="s">
         <v>41</v>
       </c>
@@ -1042,7 +1046,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" t="s">
         <v>41</v>
       </c>
@@ -1056,7 +1060,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" t="s">
         <v>41</v>
       </c>
@@ -1070,7 +1074,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" t="s">
         <v>40</v>
       </c>
@@ -1084,7 +1088,7 @@
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" t="s">
         <v>40</v>
       </c>
@@ -1098,7 +1102,7 @@
         <v>0.52500000000000002</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" t="s">
         <v>40</v>
       </c>
@@ -1112,7 +1116,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" t="s">
         <v>40</v>
       </c>
@@ -1126,7 +1130,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" t="s">
         <v>40</v>
       </c>
@@ -1140,7 +1144,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" t="s">
         <v>37</v>
       </c>
@@ -1154,7 +1158,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" t="s">
         <v>37</v>
       </c>
@@ -1168,7 +1172,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" t="s">
         <v>37</v>
       </c>
@@ -1182,7 +1186,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" t="s">
         <v>37</v>
       </c>
@@ -1196,7 +1200,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" t="s">
         <v>43</v>
       </c>
@@ -1210,7 +1214,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" t="s">
         <v>43</v>
       </c>
@@ -1224,7 +1228,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" t="s">
         <v>43</v>
       </c>
@@ -1238,7 +1242,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" t="s">
         <v>43</v>
       </c>
@@ -1252,7 +1256,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" t="s">
         <v>42</v>
       </c>
@@ -1266,7 +1270,7 @@
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" t="s">
         <v>42</v>
       </c>
@@ -1280,7 +1284,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" t="s">
         <v>42</v>
       </c>
@@ -1294,7 +1298,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" t="s">
         <v>42</v>
       </c>
@@ -1308,7 +1312,7 @@
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" t="s">
         <v>33</v>
       </c>
@@ -1322,7 +1326,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" t="s">
         <v>33</v>
       </c>
@@ -1336,7 +1340,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" t="s">
         <v>33</v>
       </c>
@@ -1350,7 +1354,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" t="s">
         <v>33</v>
       </c>
@@ -1364,7 +1368,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" t="s">
         <v>45</v>
       </c>
@@ -1378,7 +1382,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" t="s">
         <v>45</v>
       </c>
@@ -1392,7 +1396,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" t="s">
         <v>45</v>
       </c>
@@ -1406,7 +1410,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" t="s">
         <v>44</v>
       </c>
@@ -1420,7 +1424,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" t="s">
         <v>44</v>
       </c>
@@ -1434,7 +1438,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" t="s">
         <v>44</v>
       </c>
@@ -1448,7 +1452,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" t="s">
         <v>32</v>
       </c>
@@ -1462,7 +1466,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" t="s">
         <v>32</v>
       </c>
@@ -1476,7 +1480,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" t="s">
         <v>34</v>
       </c>
@@ -1496,226 +1500,283 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="26.7109375" customWidth="1"/>
-    <col min="3" max="3" width="17" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" customWidth="1"/>
+    <col min="1" max="2" width="26.68359375" customWidth="1"/>
+    <col min="4" max="4" width="17" customWidth="1"/>
+    <col min="6" max="6" width="15.578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>4</v>
       </c>
       <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>28</v>
       </c>
-      <c r="B2">
+      <c r="B2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2">
         <v>100</v>
       </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>30</v>
       </c>
-      <c r="B3">
+      <c r="B3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3">
         <v>20000</v>
       </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>29</v>
       </c>
-      <c r="B4">
-        <v>0</v>
+      <c r="B4" t="s">
+        <v>46</v>
       </c>
       <c r="C4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>35</v>
       </c>
-      <c r="B5">
-        <v>0</v>
+      <c r="B5" t="s">
+        <v>46</v>
       </c>
       <c r="C5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>31</v>
       </c>
-      <c r="B6">
+      <c r="B6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6">
         <v>15750</v>
       </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>39</v>
       </c>
-      <c r="B7">
-        <v>0</v>
+      <c r="B7" t="s">
+        <v>46</v>
       </c>
       <c r="C7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>38</v>
       </c>
-      <c r="B8">
-        <v>0</v>
+      <c r="B8" t="s">
+        <v>46</v>
       </c>
       <c r="C8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>36</v>
       </c>
-      <c r="B9">
+      <c r="B9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9">
         <v>15750</v>
       </c>
-      <c r="C9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>41</v>
       </c>
-      <c r="B10">
-        <v>0</v>
+      <c r="B10" t="s">
+        <v>46</v>
       </c>
       <c r="C10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>40</v>
       </c>
-      <c r="B11">
-        <v>0</v>
+      <c r="B11" t="s">
+        <v>46</v>
       </c>
       <c r="C11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>37</v>
       </c>
-      <c r="B12">
+      <c r="B12" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12">
         <v>15000</v>
       </c>
-      <c r="C12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>43</v>
       </c>
-      <c r="B13">
+      <c r="B13" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13">
         <v>15000</v>
       </c>
-      <c r="C13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>42</v>
       </c>
-      <c r="B14">
-        <v>0</v>
+      <c r="B14" t="s">
+        <v>46</v>
       </c>
       <c r="C14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
         <v>33</v>
       </c>
-      <c r="B15">
+      <c r="B15" t="s">
+        <v>46</v>
+      </c>
+      <c r="C15">
         <v>500</v>
       </c>
-      <c r="C15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
         <v>45</v>
       </c>
-      <c r="B16">
-        <v>0</v>
+      <c r="B16" t="s">
+        <v>46</v>
       </c>
       <c r="C16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
         <v>44</v>
       </c>
-      <c r="B17">
-        <v>0</v>
+      <c r="B17" t="s">
+        <v>46</v>
       </c>
       <c r="C17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
         <v>32</v>
       </c>
-      <c r="B18">
+      <c r="B18" t="s">
+        <v>46</v>
+      </c>
+      <c r="C18">
         <v>500</v>
       </c>
-      <c r="C18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
         <v>34</v>
       </c>
-      <c r="B19">
-        <v>0</v>
+      <c r="B19" t="s">
+        <v>46</v>
       </c>
       <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
         <v>0</v>
       </c>
     </row>
@@ -1725,225 +1786,282 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="26.140625" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" customWidth="1"/>
+    <col min="1" max="2" width="26.15625" customWidth="1"/>
+    <col min="4" max="4" width="16.83984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>4</v>
       </c>
       <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
         <v>7</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>28</v>
       </c>
-      <c r="B2">
+      <c r="B2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2">
         <v>0.75</v>
       </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>30</v>
       </c>
-      <c r="B3">
+      <c r="B3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3">
         <v>0.75</v>
       </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>29</v>
       </c>
-      <c r="B4">
+      <c r="B4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4">
         <v>0.75</v>
       </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>35</v>
       </c>
-      <c r="B5">
+      <c r="B5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5">
         <v>0.75</v>
       </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>31</v>
       </c>
-      <c r="B6">
+      <c r="B6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6">
         <v>0.75</v>
       </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>39</v>
       </c>
-      <c r="B7">
+      <c r="B7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7">
         <v>0.75</v>
       </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>38</v>
       </c>
-      <c r="B8">
+      <c r="B8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C8">
         <v>0.75</v>
       </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>36</v>
       </c>
-      <c r="B9">
+      <c r="B9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9">
         <v>0.75</v>
       </c>
-      <c r="C9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>41</v>
       </c>
-      <c r="B10">
+      <c r="B10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10">
         <v>0.75</v>
       </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>40</v>
       </c>
-      <c r="B11">
+      <c r="B11" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11">
         <v>0.75</v>
       </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>37</v>
       </c>
-      <c r="B12">
+      <c r="B12" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12">
         <v>0.75</v>
       </c>
-      <c r="C12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>43</v>
       </c>
-      <c r="B13">
+      <c r="B13" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13">
         <v>0.75</v>
       </c>
-      <c r="C13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>42</v>
       </c>
-      <c r="B14">
+      <c r="B14" t="s">
+        <v>46</v>
+      </c>
+      <c r="C14">
         <v>0.75</v>
       </c>
-      <c r="C14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
         <v>33</v>
       </c>
-      <c r="B15">
+      <c r="B15" t="s">
+        <v>46</v>
+      </c>
+      <c r="C15">
         <v>0.75</v>
       </c>
-      <c r="C15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
         <v>45</v>
       </c>
-      <c r="B16">
+      <c r="B16" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16">
         <v>0.75</v>
       </c>
-      <c r="C16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
         <v>44</v>
       </c>
-      <c r="B17">
+      <c r="B17" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17">
         <v>0.75</v>
       </c>
-      <c r="C17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
         <v>32</v>
       </c>
-      <c r="B18">
+      <c r="B18" t="s">
+        <v>46</v>
+      </c>
+      <c r="C18">
         <v>0.75</v>
       </c>
-      <c r="C18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
         <v>34</v>
       </c>
-      <c r="B19">
-        <v>0</v>
+      <c r="B19" t="s">
+        <v>46</v>
       </c>
       <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
         <v>0</v>
       </c>
     </row>
@@ -1953,20 +2071,20 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="20.5703125" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" customWidth="1"/>
+    <col min="1" max="1" width="20.578125" customWidth="1"/>
+    <col min="2" max="2" width="11.578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -1974,7 +2092,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -1982,7 +2100,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -1990,7 +2108,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -1998,7 +2116,7 @@
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>27</v>
       </c>
@@ -2012,20 +2130,20 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="21.28515625" customWidth="1"/>
+    <col min="1" max="1" width="21.26171875" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -2033,7 +2151,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -2041,7 +2159,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>24</v>
       </c>
@@ -2049,7 +2167,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>25</v>
       </c>
@@ -2057,7 +2175,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -2065,7 +2183,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -2073,7 +2191,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -2081,7 +2199,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>19</v>
       </c>

</xml_diff>